<commit_message>
Made several changes to the forms. Having difficulty getting the Other follow-ups to show.
</commit_message>
<xml_diff>
--- a/AFNET Project/Project Progress - Travis Sondgerath.xlsx
+++ b/AFNET Project/Project Progress - Travis Sondgerath.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\AFENET\Documentation\AFNET Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DCC042-FE19-4CE1-92E6-541792B370E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39886C14-9160-4411-9025-22FD3C4DAA61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">Additional Information  </t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">Documenting progress on an ongoing basis. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soliciting feedback from CDC Nigeria. </t>
   </si>
 </sst>
 </file>
@@ -256,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -273,19 +276,10 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -298,16 +292,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -321,6 +306,27 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -612,70 +618,70 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="27" style="17" customWidth="1"/>
-    <col min="3" max="3" width="36.88671875" style="17" customWidth="1"/>
-    <col min="4" max="9" width="4" style="17" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" style="21" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5546875" style="17" customWidth="1"/>
-    <col min="12" max="12" width="46.5546875" style="17" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="17"/>
+    <col min="1" max="1" width="18.21875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27" style="12" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" style="12" customWidth="1"/>
+    <col min="4" max="9" width="4" style="12" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" style="15" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5546875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="46.5546875" style="12" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+    </row>
+    <row r="2" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" s="10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="2" t="s">
         <v>0</v>
       </c>
@@ -683,20 +689,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
@@ -726,87 +732,90 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="J6" s="17"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:11" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="J7" s="17"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="25" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="17"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:11" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="17"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="132.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="17"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>